<commit_message>
LE_10_01 Revisado con corrección de estilo. LE_07_02 En edición LE_07_07 archivos de autor
</commit_message>
<xml_diff>
--- a/seguimiento/Grado10.xlsx
+++ b/seguimiento/Grado10.xlsx
@@ -1,22 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\CienciasNaturales\seguimiento\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10826" windowHeight="2872"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28280" windowHeight="15740"/>
   </bookViews>
   <sheets>
     <sheet name="Seguimiento" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -207,132 +204,132 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -347,7 +344,7 @@
         <color theme="0"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -371,13 +368,13 @@
         <color theme="0"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
         <color theme="0"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -386,7 +383,7 @@
         <color theme="0"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
         <color theme="0"/>
@@ -398,13 +395,13 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
         <color theme="0"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
         <color theme="0"/>
@@ -413,7 +410,7 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
         <color theme="0"/>
@@ -422,7 +419,7 @@
         <color theme="0"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -441,62 +438,104 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -505,48 +544,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -609,7 +606,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -644,7 +641,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -821,7 +818,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -832,357 +829,361 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.1328125" style="1" customWidth="1"/>
-    <col min="2" max="5" width="11.19921875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.73046875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.19921875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.73046875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.19921875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="22.73046875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.19921875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="22.73046875" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.6640625" style="1"/>
+    <col min="1" max="1" width="6.1640625" style="1" customWidth="1"/>
+    <col min="2" max="5" width="11.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="22.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="35" t="s">
+    <row r="1" spans="1:12" ht="16" thickBot="1">
+      <c r="B1" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="36" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
+    </row>
+    <row r="2" spans="1:12" ht="16" thickBot="1">
+      <c r="B2" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="34"/>
-      <c r="D2" s="32"/>
-    </row>
-    <row r="3" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-    </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="37" t="s">
+      <c r="D2" s="35"/>
+    </row>
+    <row r="3" spans="1:12" ht="16" thickBot="1">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+    </row>
+    <row r="4" spans="1:12" s="2" customFormat="1" ht="16" thickBot="1">
+      <c r="A4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24" t="s">
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="24"/>
-      <c r="I4" s="25" t="s">
+      <c r="H4" s="38"/>
+      <c r="I4" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="25"/>
-      <c r="K4" s="26" t="s">
+      <c r="J4" s="39"/>
+      <c r="K4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="26"/>
-    </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" ht="29.05" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="37"/>
-      <c r="B5" s="27" t="s">
+      <c r="L4" s="31"/>
+    </row>
+    <row r="5" spans="1:12" s="3" customFormat="1" ht="29" thickBot="1">
+      <c r="A5" s="36"/>
+      <c r="B5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="29" t="s">
+      <c r="J5" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="30" t="s">
+      <c r="K5" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="30" t="s">
+      <c r="L5" s="25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="38">
+    <row r="6" spans="1:12" ht="16" thickBot="1">
+      <c r="A6" s="29">
         <v>1</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="16"/>
-    </row>
-    <row r="7" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="38">
+      <c r="B6" s="4">
+        <v>42094</v>
+      </c>
+      <c r="C6" s="5">
+        <v>42094</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="15"/>
+    </row>
+    <row r="7" spans="1:12" ht="16" thickBot="1">
+      <c r="A7" s="29">
         <v>2</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="16"/>
-    </row>
-    <row r="8" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="38">
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="15"/>
+    </row>
+    <row r="8" spans="1:12" ht="16" thickBot="1">
+      <c r="A8" s="29">
         <v>3</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="16"/>
-    </row>
-    <row r="9" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="38">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="15"/>
+    </row>
+    <row r="9" spans="1:12" ht="16" thickBot="1">
+      <c r="A9" s="29">
         <v>4</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="16"/>
-    </row>
-    <row r="10" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="38">
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="15"/>
+    </row>
+    <row r="10" spans="1:12" ht="16" thickBot="1">
+      <c r="A10" s="29">
         <v>5</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="16"/>
-    </row>
-    <row r="11" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="38">
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="15"/>
+    </row>
+    <row r="11" spans="1:12" ht="16" thickBot="1">
+      <c r="A11" s="29">
         <v>6</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="16"/>
-    </row>
-    <row r="12" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="38">
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="15"/>
+    </row>
+    <row r="12" spans="1:12" ht="16" thickBot="1">
+      <c r="A12" s="29">
         <v>7</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="16"/>
-    </row>
-    <row r="13" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="38">
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="15"/>
+    </row>
+    <row r="13" spans="1:12" ht="16" thickBot="1">
+      <c r="A13" s="29">
         <v>8</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="16"/>
-    </row>
-    <row r="14" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="38">
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="15"/>
+    </row>
+    <row r="14" spans="1:12" ht="16" thickBot="1">
+      <c r="A14" s="29">
         <v>9</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="16"/>
-    </row>
-    <row r="15" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="38">
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="15"/>
+    </row>
+    <row r="15" spans="1:12" ht="16" thickBot="1">
+      <c r="A15" s="29">
         <v>10</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="16"/>
-    </row>
-    <row r="16" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="38">
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="15"/>
+    </row>
+    <row r="16" spans="1:12" ht="16" thickBot="1">
+      <c r="A16" s="29">
         <v>11</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="16"/>
-    </row>
-    <row r="17" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="38">
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="15"/>
+    </row>
+    <row r="17" spans="1:12" ht="16" thickBot="1">
+      <c r="A17" s="29">
         <v>12</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="16"/>
-    </row>
-    <row r="18" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="38">
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="15"/>
+    </row>
+    <row r="18" spans="1:12" ht="16" thickBot="1">
+      <c r="A18" s="29">
         <v>13</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="16"/>
-    </row>
-    <row r="19" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="38">
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="15"/>
+    </row>
+    <row r="19" spans="1:12" ht="16" thickBot="1">
+      <c r="A19" s="29">
         <v>14</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="16"/>
-    </row>
-    <row r="20" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="38">
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="15"/>
+    </row>
+    <row r="20" spans="1:12" ht="16" thickBot="1">
+      <c r="A20" s="29">
         <v>15</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="16"/>
-    </row>
-    <row r="21" spans="1:12" ht="16.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="39">
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="15"/>
+    </row>
+    <row r="21" spans="1:12" ht="16" thickBot="1">
+      <c r="A21" s="30">
         <v>16</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="18"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1207,6 +1208,11 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
LE_10_02_CO finalizado con corrección de estilo. Formato de seguimiento actualizado
</commit_message>
<xml_diff>
--- a/seguimiento/Grado10.xlsx
+++ b/seguimiento/Grado10.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28280" windowHeight="15740"/>
@@ -818,7 +818,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -829,7 +829,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -949,8 +949,12 @@
       <c r="A7" s="29">
         <v>2</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
+      <c r="B7" s="4">
+        <v>42110</v>
+      </c>
+      <c r="C7" s="5">
+        <v>42110</v>
+      </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="6"/>

</xml_diff>